<commit_message>
Update Dev IV Solo Project Rubric.xlsx
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DECE6F-E2F7-4CED-8C67-DD79E5A8AB04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E43DAB-9B55-4462-9AAA-B862B3ED2D3C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,12 +114,6 @@
     <t>Before Carry</t>
   </si>
   <si>
-    <t>Student Name:</t>
-  </si>
-  <si>
-    <t>Student Git Address:</t>
-  </si>
-  <si>
     <t>All Graphics API Objects cleaned up in memory</t>
   </si>
   <si>
@@ -334,6 +328,12 @@
   </si>
   <si>
     <t>Manually adjustable camera zoom level. Must be smooth and capped to a min and max value.</t>
+  </si>
+  <si>
+    <t>Student Name: Caio Tavares</t>
+  </si>
+  <si>
+    <t>Student Git Address: https://github.com/tavac/Tavares_Caio_GFX2.git</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -945,7 +947,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -961,7 +963,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -976,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1008,10 +1010,10 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>27</v>
@@ -1024,12 +1026,12 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -1069,7 +1071,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -1097,12 +1099,12 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
@@ -1139,7 +1141,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -1170,7 +1172,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1204,7 +1206,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -1235,7 +1237,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -1269,7 +1271,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
@@ -1294,7 +1296,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5">
         <v>4</v>
@@ -1319,7 +1321,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -1344,7 +1346,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
@@ -1369,7 +1371,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5">
         <v>2</v>
@@ -1411,7 +1413,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1483,7 +1485,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5">
         <v>4</v>
@@ -1508,7 +1510,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
@@ -1533,7 +1535,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="5">
         <v>4</v>
@@ -1558,7 +1560,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" s="5">
         <v>3</v>
@@ -1583,7 +1585,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
@@ -1625,7 +1627,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1644,7 +1646,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5">
         <v>3</v>
@@ -1669,7 +1671,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -1694,7 +1696,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="5">
         <v>3</v>
@@ -1719,7 +1721,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="5">
         <v>4</v>
@@ -1744,7 +1746,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" s="5">
         <v>2</v>
@@ -1769,7 +1771,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" s="5">
         <v>3</v>
@@ -1828,7 +1830,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1847,7 +1849,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="5">
         <v>3</v>
@@ -1872,7 +1874,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
@@ -1897,7 +1899,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="5">
         <v>4</v>
@@ -1922,7 +1924,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B40" s="5">
         <v>4</v>
@@ -1947,7 +1949,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5">
         <v>4</v>
@@ -1972,7 +1974,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B42" s="5">
         <v>4</v>
@@ -1997,7 +1999,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -2022,7 +2024,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -2047,7 +2049,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -2072,7 +2074,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2150,7 +2152,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B50" s="5">
         <v>3</v>
@@ -2175,7 +2177,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51" s="5">
         <v>4</v>
@@ -2200,7 +2202,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5">
         <v>4</v>
@@ -2225,7 +2227,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B53" s="5">
         <v>4</v>
@@ -2286,7 +2288,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B56" s="5">
         <v>2</v>
@@ -2311,7 +2313,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B57" s="5">
         <v>2</v>
@@ -2336,7 +2338,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" s="5">
         <v>3</v>
@@ -2361,7 +2363,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5">
         <v>4</v>
@@ -2439,7 +2441,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B63" s="5">
         <v>2</v>
@@ -2464,7 +2466,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -2489,7 +2491,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -2514,7 +2516,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -2539,7 +2541,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B67" s="5">
         <v>4</v>
@@ -2564,7 +2566,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B68" s="5">
         <v>4</v>
@@ -2642,7 +2644,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B72" s="5">
         <v>2</v>
@@ -2667,7 +2669,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -2692,7 +2694,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B74" s="5">
         <v>2</v>
@@ -2717,7 +2719,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B75" s="5">
         <v>3</v>
@@ -2742,7 +2744,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" s="5">
         <v>2</v>
@@ -2767,7 +2769,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B77" s="5">
         <v>3</v>
@@ -2792,7 +2794,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B78" s="5">
         <v>3</v>
@@ -2851,7 +2853,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2870,7 +2872,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -2891,7 +2893,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -2912,7 +2914,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -2933,7 +2935,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2954,7 +2956,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2975,7 +2977,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -3030,7 +3032,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>18</v>
@@ -3072,7 +3074,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B92" s="6">
         <v>1</v>
@@ -3118,7 +3120,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -3212,7 +3214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Lights! Camera! Quantum leaping!
Lights + dTime = party mode.
Camera looks around but is paralyzed from the Eye down, dont AT me.
Models quantum leap in and out of scene.
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1A3E61-2763-46A7-814A-F58C10766E23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AA93180-FB3A-44EB-BC24-76F8E6097B67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,15 +21,12 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -334,6 +332,9 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/tavac/Tavares_Caio_GFX2.git</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -927,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1043,9 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -1496,7 +1499,9 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
@@ -1657,7 +1662,9 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
@@ -3270,11 +3277,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3287,11 +3289,6 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3304,10 +3301,5 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
no depth, worldy barrel roll, textures...damn textures
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AA93180-FB3A-44EB-BC24-76F8E6097B67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C58CD-0F66-4128-9D5B-0EAA9A05C977}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -928,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -3221,7 +3220,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>